<commit_message>
Updated weapon classes, added more logic for transitioning between menus
</commit_message>
<xml_diff>
--- a/Weapon List.xlsx
+++ b/Weapon List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\17105519\Blacksmith\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47849B8E-C239-4C4B-89FC-11BBF34F0CF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B818F57-5DEF-4BFE-A621-000B8355840A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{4A0F80E6-59DA-43FF-BA97-8174D96CED20}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Sharpness</t>
   </si>
   <si>
-    <t>Material</t>
-  </si>
-  <si>
     <t>Defense</t>
   </si>
   <si>
@@ -78,6 +75,54 @@
   </si>
   <si>
     <t>Scythe</t>
+  </si>
+  <si>
+    <t>Cross Guard</t>
+  </si>
+  <si>
+    <t>Guard</t>
+  </si>
+  <si>
+    <t>Wide Guard</t>
+  </si>
+  <si>
+    <t>Pommel</t>
+  </si>
+  <si>
+    <t>Handle</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Rod</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Heavy</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Sharp</t>
+  </si>
+  <si>
+    <t>Blunt</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Slow</t>
   </si>
 </sst>
 </file>
@@ -119,7 +164,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -130,6 +179,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BDA341F-33A2-427E-92A1-FBDF7ACED612}" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0">
+  <autoFilter ref="A1:H13" xr:uid="{DD308456-DDEF-44FB-9A7D-E8AA701F4B76}"/>
+  <sortState ref="A2:H13">
+    <sortCondition descending="1" ref="H1:H13"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{4ABE84F5-E1F9-4162-9A90-D5A0FC9D2985}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{6B2BD6D0-B6FC-45AC-9E6C-FC7FE4CCB62E}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{AE7BBFFD-03A9-4C94-85CE-41CEA80E979C}" name="Weight"/>
+    <tableColumn id="5" xr3:uid="{C1EAE99B-CBA2-4122-89DF-00D1008FCC3B}" name="Length"/>
+    <tableColumn id="6" xr3:uid="{3F471884-6572-4571-A7B8-238DE21A2D3B}" name="Sharpness"/>
+    <tableColumn id="7" xr3:uid="{0556FF29-8389-4012-93E0-092C12EC9C51}" name="Defense"/>
+    <tableColumn id="8" xr3:uid="{F649C125-EE62-48C6-8070-3CDA0D9BEDD1}" name="Handling"/>
+    <tableColumn id="3" xr3:uid="{ABE15C5D-92D8-48E9-BF72-5191644C0DB4}" name="Damage" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C570A0-EF96-4B02-8EF9-F707650C02E9}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,13 +513,13 @@
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,147 +527,388 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H11">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
+      <c r="H13">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Random Hilt Generation and Selection
</commit_message>
<xml_diff>
--- a/Weapon List.xlsx
+++ b/Weapon List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\17105519\Blacksmith\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1D2618-F37C-48F6-87E5-46AB56521F43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B042C65C-B897-4C3F-8086-43DFCE089467}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{4A0F80E6-59DA-43FF-BA97-8174D96CED20}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Guard</t>
   </si>
   <si>
-    <t>Wide Guard</t>
-  </si>
-  <si>
     <t>Pommel</t>
   </si>
   <si>
@@ -95,7 +92,46 @@
     <t>Staff</t>
   </si>
   <si>
-    <t>Rod</t>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>French Guard</t>
+  </si>
+  <si>
+    <t>T Guard</t>
+  </si>
+  <si>
+    <t>Y Guard</t>
+  </si>
+  <si>
+    <t>Ornamental Dagger</t>
+  </si>
+  <si>
+    <t>2H Pommel</t>
+  </si>
+  <si>
+    <t>Axe Guard</t>
+  </si>
+  <si>
+    <t>Battleaxe</t>
+  </si>
+  <si>
+    <t>Flamberg</t>
+  </si>
+  <si>
+    <t>Hilt</t>
+  </si>
+  <si>
+    <t>Longsword</t>
+  </si>
+  <si>
+    <t>Thin 2H</t>
+  </si>
+  <si>
+    <t>Thin Pommel</t>
+  </si>
+  <si>
+    <t>Zweihander</t>
   </si>
 </sst>
 </file>
@@ -131,8 +167,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,10 +192,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BDA341F-33A2-427E-92A1-FBDF7ACED612}" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0">
-  <autoFilter ref="A1:H13" xr:uid="{DD308456-DDEF-44FB-9A7D-E8AA701F4B76}"/>
-  <sortState ref="A2:H13">
-    <sortCondition descending="1" ref="H1:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BDA341F-33A2-427E-92A1-FBDF7ACED612}" name="Table1" displayName="Table1" ref="A1:H24" totalsRowShown="0">
+  <autoFilter ref="A1:H24" xr:uid="{DD308456-DDEF-44FB-9A7D-E8AA701F4B76}"/>
+  <sortState ref="A2:H24">
+    <sortCondition descending="1" ref="H1:H24"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4ABE84F5-E1F9-4162-9A90-D5A0FC9D2985}" name="Name"/>
@@ -473,15 +510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C570A0-EF96-4B02-8EF9-F707650C02E9}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
@@ -520,17 +557,17 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -538,25 +575,25 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>22.5</v>
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -567,23 +604,23 @@
       <c r="G3">
         <v>4</v>
       </c>
-      <c r="H3">
-        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>19</v>
+      <c r="H3" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -592,25 +629,25 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>11</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -619,79 +656,79 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>10</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -700,52 +737,52 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>5.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>5</v>
       </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
       <c r="H9">
         <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -754,25 +791,25 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>1</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -781,65 +818,362 @@
         <v>0</v>
       </c>
       <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
         <v>7</v>
-      </c>
-      <c r="H11">
-        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="H12" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
-        <v>0</v>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23" s="1">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f>Table1[[#This Row],[Length]]/2 * Table1[[#This Row],[Weight]] + Table1[[#This Row],[Sharpness]]*5</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>